<commit_message>
Database updated files removed from repo
</commit_message>
<xml_diff>
--- a/other/store_features.xlsx
+++ b/other/store_features.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodo/Documents/Developer/WebDev/React/Watch_Store/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE67EB54-B17E-AA4B-8B70-38F9A57445B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07F0DCB-73E1-B345-9960-7FAD92F016E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="1760" windowWidth="43140" windowHeight="28360" xr2:uid="{7C02AD0A-9C52-634F-9977-20B801EA9689}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="32000" activeTab="1" xr2:uid="{7C02AD0A-9C52-634F-9977-20B801EA9689}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="34">
   <si>
     <t>Admin</t>
   </si>
@@ -130,6 +131,12 @@
   </si>
   <si>
     <t>Add</t>
+  </si>
+  <si>
+    <t>userid</t>
+  </si>
+  <si>
+    <t>storeid</t>
   </si>
 </sst>
 </file>
@@ -372,6 +379,39 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -402,88 +442,55 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -802,11 +809,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7514F5A-3E92-CB47-8AFF-B2C8F804A27C}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -815,30 +822,30 @@
     <col min="2" max="2" width="6.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" style="1" customWidth="1"/>
     <col min="4" max="7" width="16.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="68.1640625" style="40" customWidth="1"/>
+    <col min="8" max="8" width="68.1640625" style="10" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="38" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="30" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
@@ -851,13 +858,13 @@
       <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="38"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -871,11 +878,11 @@
       <c r="G3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="39"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
@@ -889,11 +896,11 @@
         <v>13</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="39"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
@@ -907,11 +914,11 @@
         <v>13</v>
       </c>
       <c r="G5" s="2"/>
-      <c r="H5" s="39"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
@@ -925,11 +932,11 @@
         <v>13</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="39"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="32"/>
+      <c r="B7" s="31" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -941,11 +948,11 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="39"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
@@ -955,11 +962,11 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="39"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
@@ -969,11 +976,11 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="39"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
-      <c r="B10" s="19"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
@@ -983,13 +990,13 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="39"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="46" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1003,11 +1010,11 @@
         <v>13</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="39"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="33"/>
-      <c r="B12" s="34"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1019,11 +1026,11 @@
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="39"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="33"/>
-      <c r="B13" s="34"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="46"/>
       <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
@@ -1035,11 +1042,11 @@
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="39"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="33"/>
-      <c r="B14" s="34"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
@@ -1051,11 +1058,11 @@
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="39"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34" t="s">
+      <c r="A15" s="45"/>
+      <c r="B15" s="46" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1067,11 +1074,11 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="39"/>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1087,11 +1094,11 @@
       <c r="G16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="39"/>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="33"/>
-      <c r="B17" s="34"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1101,11 +1108,11 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="39"/>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="2" t="s">
         <v>10</v>
       </c>
@@ -1115,13 +1122,13 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="39"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="42" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1139,11 +1146,11 @@
       <c r="G19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="39"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
-      <c r="B20" s="31"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="43"/>
       <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
@@ -1159,11 +1166,11 @@
       <c r="G20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="39"/>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="28"/>
-      <c r="B21" s="31"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
@@ -1175,11 +1182,11 @@
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="39"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="28"/>
-      <c r="B22" s="31"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="43"/>
       <c r="C22" s="2" t="s">
         <v>9</v>
       </c>
@@ -1193,11 +1200,11 @@
         <v>13</v>
       </c>
       <c r="G22" s="2"/>
-      <c r="H22" s="39"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="28"/>
-      <c r="B23" s="32"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="44"/>
       <c r="C23" s="2" t="s">
         <v>10</v>
       </c>
@@ -1211,11 +1218,11 @@
         <v>13</v>
       </c>
       <c r="G23" s="2"/>
-      <c r="H23" s="39"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="28"/>
-      <c r="B24" s="30" t="s">
+      <c r="A24" s="40"/>
+      <c r="B24" s="42" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1233,11 +1240,11 @@
       <c r="G24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H24" s="39"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="28"/>
-      <c r="B25" s="31"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="43"/>
       <c r="C25" s="2" t="s">
         <v>7</v>
       </c>
@@ -1247,11 +1254,11 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="39"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="28"/>
-      <c r="B26" s="31"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="43"/>
       <c r="C26" s="2" t="s">
         <v>8</v>
       </c>
@@ -1261,11 +1268,11 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="39"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="28"/>
-      <c r="B27" s="31"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="43"/>
       <c r="C27" s="2" t="s">
         <v>9</v>
       </c>
@@ -1275,11 +1282,11 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="39"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
-      <c r="B28" s="32"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="44"/>
       <c r="C28" s="2" t="s">
         <v>10</v>
       </c>
@@ -1289,13 +1296,13 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="39"/>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1313,11 +1320,11 @@
       <c r="G29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="39"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="25"/>
-      <c r="B30" s="22"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="34"/>
       <c r="C30" s="2" t="s">
         <v>7</v>
       </c>
@@ -1333,11 +1340,11 @@
       <c r="G30" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="39"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="25"/>
-      <c r="B31" s="22"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="34"/>
       <c r="C31" s="2" t="s">
         <v>8</v>
       </c>
@@ -1349,11 +1356,11 @@
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="39"/>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="25"/>
-      <c r="B32" s="22"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="34"/>
       <c r="C32" s="2" t="s">
         <v>9</v>
       </c>
@@ -1367,11 +1374,11 @@
         <v>13</v>
       </c>
       <c r="G32" s="2"/>
-      <c r="H32" s="39"/>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="25"/>
-      <c r="B33" s="23"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="35"/>
       <c r="C33" s="2" t="s">
         <v>10</v>
       </c>
@@ -1385,11 +1392,11 @@
         <v>13</v>
       </c>
       <c r="G33" s="2"/>
-      <c r="H33" s="39"/>
+      <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="25"/>
-      <c r="B34" s="21" t="s">
+      <c r="A34" s="37"/>
+      <c r="B34" s="33" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -1407,11 +1414,11 @@
       <c r="G34" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H34" s="39"/>
+      <c r="H34" s="9"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="25"/>
-      <c r="B35" s="22"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="34"/>
       <c r="C35" s="2" t="s">
         <v>7</v>
       </c>
@@ -1423,11 +1430,11 @@
       <c r="G35" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H35" s="39"/>
+      <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="25"/>
-      <c r="B36" s="22"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="2" t="s">
         <v>8</v>
       </c>
@@ -1437,11 +1444,11 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="39"/>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="25"/>
-      <c r="B37" s="22"/>
+      <c r="A37" s="37"/>
+      <c r="B37" s="34"/>
       <c r="C37" s="2" t="s">
         <v>9</v>
       </c>
@@ -1451,11 +1458,11 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="39"/>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="26"/>
-      <c r="B38" s="23"/>
+      <c r="A38" s="38"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="2" t="s">
         <v>10</v>
       </c>
@@ -1465,13 +1472,13 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="39"/>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -1489,13 +1496,13 @@
       <c r="G39" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H39" s="39" t="s">
+      <c r="H39" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="36"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="2" t="s">
         <v>22</v>
       </c>
@@ -1505,13 +1512,13 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="39" t="s">
+      <c r="H40" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="36"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="12"/>
       <c r="C41" s="2" t="s">
         <v>9</v>
       </c>
@@ -1525,13 +1532,13 @@
         <v>13</v>
       </c>
       <c r="G41" s="2"/>
-      <c r="H41" s="39" t="s">
+      <c r="H41" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="37"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="13"/>
       <c r="C42" s="2" t="s">
         <v>10</v>
       </c>
@@ -1545,13 +1552,13 @@
         <v>13</v>
       </c>
       <c r="G42" s="2"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="10"/>
-      <c r="B43" s="35" t="s">
+      <c r="A43" s="21"/>
+      <c r="B43" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -1569,13 +1576,13 @@
       <c r="G43" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H43" s="39" t="s">
+      <c r="H43" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="10"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="21"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="2" t="s">
         <v>22</v>
       </c>
@@ -1591,13 +1598,13 @@
       <c r="G44" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H44" s="39" t="s">
+      <c r="H44" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="10"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="21"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="2" t="s">
         <v>9</v>
       </c>
@@ -1607,13 +1614,13 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
-      <c r="H45" s="39" t="s">
+      <c r="H45" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="11"/>
-      <c r="B46" s="37"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="2" t="s">
         <v>10</v>
       </c>
@@ -1623,15 +1630,15 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
-      <c r="H46" s="39" t="s">
+      <c r="H46" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B47" s="44" t="s">
+      <c r="B47" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -1647,11 +1654,11 @@
         <v>13</v>
       </c>
       <c r="G47" s="2"/>
-      <c r="H47" s="39"/>
+      <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="42"/>
-      <c r="B48" s="45"/>
+      <c r="A48" s="18"/>
+      <c r="B48" s="15"/>
       <c r="C48" s="2" t="s">
         <v>31</v>
       </c>
@@ -1665,11 +1672,11 @@
         <v>13</v>
       </c>
       <c r="G48" s="2"/>
-      <c r="H48" s="39"/>
+      <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="42"/>
-      <c r="B49" s="45"/>
+      <c r="A49" s="18"/>
+      <c r="B49" s="15"/>
       <c r="C49" s="2" t="s">
         <v>9</v>
       </c>
@@ -1683,11 +1690,11 @@
         <v>13</v>
       </c>
       <c r="G49" s="2"/>
-      <c r="H49" s="39"/>
+      <c r="H49" s="9"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="42"/>
-      <c r="B50" s="46"/>
+      <c r="A50" s="18"/>
+      <c r="B50" s="16"/>
       <c r="C50" s="2" t="s">
         <v>10</v>
       </c>
@@ -1701,11 +1708,11 @@
         <v>13</v>
       </c>
       <c r="G50" s="2"/>
-      <c r="H50" s="39"/>
+      <c r="H50" s="9"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="42"/>
-      <c r="B51" s="44" t="s">
+      <c r="A51" s="18"/>
+      <c r="B51" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -1717,11 +1724,11 @@
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="39"/>
+      <c r="H51" s="9"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="42"/>
-      <c r="B52" s="45"/>
+      <c r="A52" s="18"/>
+      <c r="B52" s="15"/>
       <c r="C52" s="2" t="s">
         <v>31</v>
       </c>
@@ -1731,11 +1738,11 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
-      <c r="H52" s="39"/>
+      <c r="H52" s="9"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="42"/>
-      <c r="B53" s="45"/>
+      <c r="A53" s="18"/>
+      <c r="B53" s="15"/>
       <c r="C53" s="2" t="s">
         <v>9</v>
       </c>
@@ -1745,11 +1752,11 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="39"/>
+      <c r="H53" s="9"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="43"/>
-      <c r="B54" s="46"/>
+      <c r="A54" s="19"/>
+      <c r="B54" s="16"/>
       <c r="C54" s="2" t="s">
         <v>10</v>
       </c>
@@ -1759,32 +1766,71 @@
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
-      <c r="H54" s="39"/>
+      <c r="H54" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="A29:A38"/>
+    <mergeCell ref="A19:A28"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="A3:A10"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="B43:B46"/>
     <mergeCell ref="B47:B50"/>
     <mergeCell ref="B51:B54"/>
     <mergeCell ref="A47:A54"/>
     <mergeCell ref="A39:A46"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="A29:A38"/>
-    <mergeCell ref="A19:A28"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B15:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3913743F-1729-0749-9756-E338D4D07135}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>